<commit_message>
Counter for repeated StartLocations
</commit_message>
<xml_diff>
--- a/RouteVisualizationData.xlsx
+++ b/RouteVisualizationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\HeatMap\geo_Jakubiec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295E5286-DA4E-4DAE-89D4-5C6E8F63EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3A73F9-64BD-413E-9686-08BE51075A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2F3686D1-0F06-4A3D-B745-F95CFAFEAE70}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="238">
   <si>
     <t>Burgemeester Lemmensstraat 152 6163 JR, Geleen</t>
   </si>
@@ -821,7 +821,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -876,6 +906,26 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1235,10 +1285,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982ADBEB-26D6-4671-B50D-111DA5BCB48A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,22 +1377,122 @@
         <v>98</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B14:B1048576">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="A2:A3 A11:A12">
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4:A10">
+    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1 B22:B1048576">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Dobrowo 29, Dobrowo"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3 A11:A12">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3 B12:B13">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  <conditionalFormatting sqref="B4:B10">
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A10">
+  <conditionalFormatting sqref="B11:B18">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:B21">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B11">
+  <conditionalFormatting sqref="A21">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1355,8 +1505,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C234"/>
   <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:A110"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A178" sqref="A178:A185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3820,7 +3970,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New locations in excel to be checked
</commit_message>
<xml_diff>
--- a/RouteVisualizationData.xlsx
+++ b/RouteVisualizationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr updateLinks="always" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\HeatMap\geo_Jakubiec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ottoworkforcebv-my.sharepoint.com/personal/pjakubiec_ottoworkforce_eu/Documents/Documenten/HeatMap Project/geo_Jakubiec/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3A73F9-64BD-413E-9686-08BE51075A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{6A3A73F9-64BD-413E-9686-08BE51075A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7813095A-B4A0-421B-B81F-29ACEE6530DB}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2F3686D1-0F06-4A3D-B745-F95CFAFEAE70}"/>
+    <workbookView xWindow="42780" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{2F3686D1-0F06-4A3D-B745-F95CFAFEAE70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="243">
   <si>
     <t>Burgemeester Lemmensstraat 152 6163 JR, Geleen</t>
   </si>
@@ -754,6 +754,21 @@
   </si>
   <si>
     <t>Vorstengrafdonk 63 5342 LW, Oss</t>
+  </si>
+  <si>
+    <t>Goudplevier 79 5348 ZB, Oss</t>
+  </si>
+  <si>
+    <t>Leeuwerikstraat 5 5348 XA, Oss</t>
+  </si>
+  <si>
+    <t>Staringstraat 320 5343 GN, Oss</t>
+  </si>
+  <si>
+    <t>Slingenbergstraat 10 5344 KL, Oss</t>
+  </si>
+  <si>
+    <t>Markermeer 1 5347 JM, Oss</t>
   </si>
 </sst>
 </file>
@@ -821,27 +836,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -906,6 +901,16 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1285,10 +1290,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982ADBEB-26D6-4671-B50D-111DA5BCB48A}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,204 +1302,224 @@
     <col min="2" max="2" width="55.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>238</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>239</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>240</v>
       </c>
       <c r="B11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>46</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>114</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>241</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
+      <c r="B24" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>218</v>
+      </c>
+      <c r="B26" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A3 A11:A12">
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4:A10">
-    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1 B22:B1048576">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
-      <formula>"Dobrowo 29, Dobrowo"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B10">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11:B18">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20:B21">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3970,7 +3995,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add nr of Passengers in one trip
</commit_message>
<xml_diff>
--- a/RouteVisualizationData.xlsx
+++ b/RouteVisualizationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr updateLinks="always" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ottoworkforcebv-my.sharepoint.com/personal/pjakubiec_ottoworkforce_eu/Documents/Documenten/HeatMap Project/geo_Jakubiec/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\HeatMap\geo_Jakubiec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{6A3A73F9-64BD-413E-9686-08BE51075A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7813095A-B4A0-421B-B81F-29ACEE6530DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2011543B-9990-453A-9F79-AF01F0967986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42780" yWindow="5535" windowWidth="28800" windowHeight="15345" xr2:uid="{2F3686D1-0F06-4A3D-B745-F95CFAFEAE70}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2F3686D1-0F06-4A3D-B745-F95CFAFEAE70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="239">
   <si>
     <t>Burgemeester Lemmensstraat 152 6163 JR, Geleen</t>
   </si>
@@ -756,19 +756,7 @@
     <t>Vorstengrafdonk 63 5342 LW, Oss</t>
   </si>
   <si>
-    <t>Goudplevier 79 5348 ZB, Oss</t>
-  </si>
-  <si>
-    <t>Leeuwerikstraat 5 5348 XA, Oss</t>
-  </si>
-  <si>
-    <t>Staringstraat 320 5343 GN, Oss</t>
-  </si>
-  <si>
-    <t>Slingenbergstraat 10 5344 KL, Oss</t>
-  </si>
-  <si>
-    <t>Markermeer 1 5347 JM, Oss</t>
+    <t>NrPassengers</t>
   </si>
 </sst>
 </file>
@@ -836,7 +824,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -854,53 +842,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1293,13 +1234,14 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1309,217 +1251,309 @@
       <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1"/>
+      <c r="C1" s="2" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>181</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
-        <v>242</v>
+        <v>181</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>160</v>
       </c>
       <c r="B6" t="s">
-        <v>242</v>
+        <v>181</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>181</v>
+      </c>
+      <c r="C8">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>163</v>
       </c>
       <c r="B9" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="B10" t="s">
-        <v>242</v>
+        <v>181</v>
+      </c>
+      <c r="C10">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>240</v>
+        <v>181</v>
       </c>
       <c r="B11" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="C11">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>242</v>
+        <v>181</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>183</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="C13">
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>233</v>
       </c>
       <c r="B14" t="s">
-        <v>242</v>
+        <v>181</v>
+      </c>
+      <c r="C14">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>184</v>
       </c>
       <c r="B15" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>188</v>
+      </c>
+      <c r="B19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>189</v>
+      </c>
+      <c r="B20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C21">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>191</v>
+      </c>
+      <c r="B22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B20" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>241</v>
-      </c>
-      <c r="B21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B22" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="B23" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>218</v>
+        <v>193</v>
       </c>
       <c r="B24" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="B25" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="C25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="B26" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="B27" t="s">
-        <v>242</v>
+        <v>233</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:A9">
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:A24">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A25:A27">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1530,8 +1564,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C234"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="A178" sqref="A178:A185"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A204" activeCellId="1" sqref="A207 A204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>